<commit_message>
Rebuilt Panel and loop
</commit_message>
<xml_diff>
--- a/scintillator.xlsx
+++ b/scintillator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawaiz\Documents\3D\Inventor\SiPm ScintillatorTest Kit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawaiz\Documents\data\projects\scintillatorPanel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>ScintillatorThickness</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>MountingScrewDepth</t>
+  </si>
+  <si>
+    <t>LoopLength</t>
   </si>
 </sst>
 </file>
@@ -419,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>145</v>
+        <v>290</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -602,7 +605,7 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
@@ -682,6 +685,17 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>140</v>
+      </c>
+      <c r="C24" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
7mm scintilator, fiber slopes down to meet with center of panel
</commit_message>
<xml_diff>
--- a/scintillator.xlsx
+++ b/scintillator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawaiz\Documents\data\projects\scintillatorPanel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawaiz\OneDrive\projects\scintillatorPanel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>ScintillatorThickness</t>
   </si>
@@ -35,12 +35,6 @@
     <t>OpticalFiberClearence</t>
   </si>
   <si>
-    <t>SmallTrackDiameter</t>
-  </si>
-  <si>
-    <t>LargeTrackRatio</t>
-  </si>
-  <si>
     <t>ul</t>
   </si>
   <si>
@@ -59,36 +53,9 @@
     <t>ShallowTrackDepth</t>
   </si>
   <si>
-    <t>MPPCClearence</t>
-  </si>
-  <si>
-    <t>MPPCSensorClearence</t>
-  </si>
-  <si>
-    <t>MPPCSensorOffsett</t>
-  </si>
-  <si>
-    <t>MPPCWidth</t>
-  </si>
-  <si>
-    <t>MPPCHeight</t>
-  </si>
-  <si>
     <t>FiberEdgeOffsett</t>
   </si>
   <si>
-    <t>MPPCDepth</t>
-  </si>
-  <si>
-    <t>LongFiberAngle</t>
-  </si>
-  <si>
-    <t>ShortFiberAngle</t>
-  </si>
-  <si>
-    <t>deg</t>
-  </si>
-  <si>
     <t>LoopLargeTrackRatio</t>
   </si>
   <si>
@@ -101,10 +68,10 @@
     <t>MountingScrewOffsett</t>
   </si>
   <si>
-    <t>MountingScrewDepth</t>
-  </si>
-  <si>
     <t>LoopLength</t>
+  </si>
+  <si>
+    <t>DeepTrackDepth</t>
   </si>
 </sst>
 </file>
@@ -422,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +408,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -449,10 +416,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -460,32 +427,32 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>175</v>
-      </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -493,10 +460,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -504,199 +471,89 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>145</v>
+        <f>B1+(2*B3)</f>
+        <v>1.2</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B8">
-        <v>145</v>
+        <f>B2/2+(B7/2)</f>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <f>B1+(2*B3)</f>
-        <v>1.3</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>7.4999999999999997E-2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>1.45</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <f>0.5+1+0.605</f>
-        <v>2.105</v>
+        <v>0.5</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>5.9</v>
+        <v>12.5</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>6.55</v>
+        <v>140</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18">
-        <v>78</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20">
-        <v>90</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21">
-        <v>0.5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22">
-        <v>20</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24">
-        <v>140</v>
-      </c>
-      <c r="C24" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shaped to a close approximation no fillet
</commit_message>
<xml_diff>
--- a/scintillator.xlsx
+++ b/scintillator.xlsx
@@ -392,7 +392,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +517,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
finger scintintlator with silvering and rubber
</commit_message>
<xml_diff>
--- a/scintillator.xlsx
+++ b/scintillator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawaiz\OneDrive\projects\scintillatorPanel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawai\OneDrive\projects\scintillatorPanel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>ScintillatorThickness</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>DeepTrackDepth</t>
+  </si>
+  <si>
+    <t>silveringThickness</t>
+  </si>
+  <si>
+    <t>rubberizedCoating</t>
   </si>
 </sst>
 </file>
@@ -389,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,7 +422,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -449,7 +455,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>145</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -460,7 +466,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>145</v>
+        <v>200</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -484,7 +490,7 @@
       </c>
       <c r="B8">
         <f>B2/2+(B7/2)</f>
-        <v>4.0999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -539,7 +545,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>12.5</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -553,6 +559,28 @@
         <v>140</v>
       </c>
       <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>0.2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>0.5</v>
+      </c>
+      <c r="C16" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rebuilt most files, renamed peramters.
</commit_message>
<xml_diff>
--- a/scintillator.xlsx
+++ b/scintillator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawaiz\OneDrive\projects\scintillatorPanel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawai\OneDrive\projects\scintillatorPanel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,75 +24,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
-  <si>
-    <t>ScintillatorThickness</t>
-  </si>
-  <si>
-    <t>OpticalFiberDiameter</t>
-  </si>
-  <si>
-    <t>OpticalFiberClearence</t>
-  </si>
-  <si>
-    <t>ul</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>mm</t>
   </si>
   <si>
-    <t>ScintillatorEdgeClearence</t>
-  </si>
-  <si>
-    <t>ScintillatorWidth</t>
-  </si>
-  <si>
-    <t>ScintillatorHeight</t>
-  </si>
-  <si>
-    <t>ShallowTrackDepth</t>
-  </si>
-  <si>
-    <t>FiberEdgeOffsett</t>
-  </si>
-  <si>
-    <t>LoopLargeTrackRatio</t>
-  </si>
-  <si>
-    <t>LoopSmallTrackDiameter</t>
-  </si>
-  <si>
-    <t>FiberSensorClerence</t>
-  </si>
-  <si>
-    <t>MountingScrewOffsett</t>
-  </si>
-  <si>
-    <t>LoopLength</t>
-  </si>
-  <si>
-    <t>DeepTrackDepth</t>
-  </si>
-  <si>
     <t>silveringThickness</t>
   </si>
   <si>
     <t>rubberizedCoating</t>
   </si>
   <si>
-    <t>mppcMountDepth</t>
-  </si>
-  <si>
-    <t>in</t>
-  </si>
-  <si>
-    <t>fingerCount</t>
-  </si>
-  <si>
     <t>mil</t>
   </si>
   <si>
-    <t>millSize</t>
+    <t>Perameter</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>opticalFiberDiameter</t>
+  </si>
+  <si>
+    <t>scintillatorThickness</t>
+  </si>
+  <si>
+    <t>opticalFiberClearence</t>
+  </si>
+  <si>
+    <t>scintillatorEdgeClearence</t>
+  </si>
+  <si>
+    <t>scintillatorWidth</t>
+  </si>
+  <si>
+    <t>scintillatorHeight</t>
+  </si>
+  <si>
+    <t>shallowTrackDepth</t>
+  </si>
+  <si>
+    <t>deepTrackDepth</t>
+  </si>
+  <si>
+    <t>fiberEdgeOffsett</t>
+  </si>
+  <si>
+    <t>curvatureRadius</t>
   </si>
 </sst>
 </file>
@@ -410,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,207 +405,147 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>7.0999999999999994E-2</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <f>B1+(2*B3)</f>
-        <v>1.1419999999999999</v>
+        <v>200</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8">
-        <f>B2/2+(B7/2)</f>
-        <v>5.5709999999999997</v>
+        <f>B2+(2*B4)</f>
+        <v>1.1419999999999999</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <f>B3/2+(B8/2)</f>
+        <v>5.5709999999999997</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B10">
-        <v>1.1000000000000001</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B12">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B13">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>140</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>0.2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>20</v>
-      </c>
-      <c r="C16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <v>0.25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the design for the loopPanel, added the drawing file for it, and removed the showcase folder
</commit_message>
<xml_diff>
--- a/scintillator.xlsx
+++ b/scintillator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawaiz\OneDrive\projects\scintillatorPanel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\Projects\loop\scintillatorPanel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>ScintillatorThickness</t>
   </si>
@@ -32,18 +32,12 @@
     <t>OpticalFiberDiameter</t>
   </si>
   <si>
-    <t>OpticalFiberClearence</t>
-  </si>
-  <si>
     <t>ul</t>
   </si>
   <si>
     <t>mm</t>
   </si>
   <si>
-    <t>ScintillatorEdgeClearence</t>
-  </si>
-  <si>
     <t>ScintillatorWidth</t>
   </si>
   <si>
@@ -62,9 +56,6 @@
     <t>LoopSmallTrackDiameter</t>
   </si>
   <si>
-    <t>FiberSensorClerence</t>
-  </si>
-  <si>
     <t>MountingScrewOffsett</t>
   </si>
   <si>
@@ -72,12 +63,30 @@
   </si>
   <si>
     <t>DeepTrackDepth</t>
+  </si>
+  <si>
+    <t>CornerCut</t>
+  </si>
+  <si>
+    <t>inch</t>
+  </si>
+  <si>
+    <t>OpticalFiberClearance</t>
+  </si>
+  <si>
+    <t>ScintillatorEdgeClearance</t>
+  </si>
+  <si>
+    <t>FiberSensorClerance</t>
+  </si>
+  <si>
+    <t>(.5 in)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -389,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,7 +409,7 @@
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -408,152 +417,166 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>12.7</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>0.1</v>
       </c>
       <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5">
+        <v>5.75</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6">
+        <v>5.75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
-      </c>
-      <c r="B5">
-        <v>145</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>145</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
       </c>
       <c r="B7">
         <f>B1+(2*B3)</f>
         <v>1.2</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <f>B2/2+(B7/2)</f>
-        <v>4.0999999999999996</v>
+        <v>6.9499999999999993</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>1.1000000000000001</v>
+        <v>1.25</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>0.5</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <v>12.5</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>140</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed clearance for fiber
</commit_message>
<xml_diff>
--- a/scintillator.xlsx
+++ b/scintillator.xlsx
@@ -401,7 +401,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +439,7 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -484,7 +484,7 @@
       </c>
       <c r="B7">
         <f>B1+(2*B3)</f>
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -496,7 +496,7 @@
       </c>
       <c r="B8">
         <f>B2/2+(B7/2)</f>
-        <v>6.9499999999999993</v>
+        <v>6.85</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -518,7 +518,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -573,7 +573,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Added a Readme, yay
</commit_message>
<xml_diff>
--- a/scintillator.xlsx
+++ b/scintillator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawai\OneDrive\projects\scintillatorPanel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02be13960f358456/projects/scintillatorPanel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -205,6 +205,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -240,6 +257,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">

</xml_diff>

<commit_message>
Rebuilt with cut corner
</commit_message>
<xml_diff>
--- a/scintillator.xlsx
+++ b/scintillator.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawaiz\Documents\data\projects\scintillatorPanel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\oneDrive\projects\scintillatorPanel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>ScintillatorThickness</t>
   </si>
@@ -59,36 +59,9 @@
     <t>ShallowTrackDepth</t>
   </si>
   <si>
-    <t>MPPCClearence</t>
-  </si>
-  <si>
-    <t>MPPCSensorClearence</t>
-  </si>
-  <si>
-    <t>MPPCSensorOffsett</t>
-  </si>
-  <si>
-    <t>MPPCWidth</t>
-  </si>
-  <si>
-    <t>MPPCHeight</t>
-  </si>
-  <si>
     <t>FiberEdgeOffsett</t>
   </si>
   <si>
-    <t>MPPCDepth</t>
-  </si>
-  <si>
-    <t>LongFiberAngle</t>
-  </si>
-  <si>
-    <t>ShortFiberAngle</t>
-  </si>
-  <si>
-    <t>deg</t>
-  </si>
-  <si>
     <t>LoopLargeTrackRatio</t>
   </si>
   <si>
@@ -98,19 +71,28 @@
     <t>FiberSensorClerence</t>
   </si>
   <si>
-    <t>MountingScrewOffsett</t>
-  </si>
-  <si>
-    <t>MountingScrewDepth</t>
-  </si>
-  <si>
-    <t>LoopLength</t>
+    <t>cornerChamfer</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>mountingSpacing</t>
+  </si>
+  <si>
+    <t>silveringThickness</t>
+  </si>
+  <si>
+    <t>rubberizedCoating</t>
+  </si>
+  <si>
+    <t>mil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -235,6 +217,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -270,6 +269,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -422,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +554,7 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>7.4999999999999997E-2</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -549,10 +565,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>1.45</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -560,8 +576,7 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <f>0.5+1+0.605</f>
-        <v>2.105</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -572,7 +587,7 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>5.9</v>
+        <v>0.5</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -580,10 +595,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>6.55</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -591,21 +606,21 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>16</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
@@ -613,90 +628,13 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18">
-        <v>78</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20">
-        <v>90</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21">
-        <v>0.5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22">
-        <v>20</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24">
-        <v>140</v>
-      </c>
-      <c r="C24" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on blender model, updated to remove 3d cut and change size to 200^2
</commit_message>
<xml_diff>
--- a/scintillator.xlsx
+++ b/scintillator.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\oneDrive\projects\scintillatorPanel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\oneDrive\projects\physics\muonTelescope\scintillatorPanel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_A346E5C2711A111ED5825FAE551B7E41938DBFA6" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{E1D9E4D2-A58C-47FF-A88E-688228982B40}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12570"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>ScintillatorThickness</t>
   </si>
@@ -35,12 +42,6 @@
     <t>OpticalFiberClearence</t>
   </si>
   <si>
-    <t>SmallTrackDiameter</t>
-  </si>
-  <si>
-    <t>LargeTrackRatio</t>
-  </si>
-  <si>
     <t>ul</t>
   </si>
   <si>
@@ -54,9 +55,6 @@
   </si>
   <si>
     <t>ScintillatorHeight</t>
-  </si>
-  <si>
-    <t>ShallowTrackDepth</t>
   </si>
   <si>
     <t>FiberEdgeOffsett</t>
@@ -92,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -437,19 +435,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -457,10 +455,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -468,10 +466,10 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -479,162 +477,128 @@
         <v>0.15</v>
       </c>
       <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>175</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
       <c r="B5">
-        <v>3</v>
+        <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>200</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>145</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>145</v>
+        <v>1.5</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <f>B1+(2*B3)</f>
-        <v>1.3</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>100</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
         <v>17</v>
-      </c>
-      <c r="B14">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16">
-        <v>0.2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>